<commit_message>
commiting files to local system
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Create RTI Employees201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Create RTI Employees201718.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
   <si>
     <t>FirstName</t>
   </si>
@@ -246,10 +246,13 @@
     <t>Regular work pattern - days</t>
   </si>
   <si>
-    <t>RTI employee 1002</t>
-  </si>
-  <si>
-    <t>rtiemployee1003@xcdgmail.com</t>
+    <t>16</t>
+  </si>
+  <si>
+    <t>rtiemployee1014@xcdgmail.com</t>
+  </si>
+  <si>
+    <t>RTI employee 1014</t>
   </si>
 </sst>
 </file>
@@ -715,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +895,7 @@
         <v>68</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>74</v>
@@ -924,8 +927,8 @@
       <c r="M2" s="4">
         <v>5</v>
       </c>
-      <c r="N2" s="4">
-        <v>40</v>
+      <c r="N2" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>41</v>

</xml_diff>